<commit_message>
Added write test #5
</commit_message>
<xml_diff>
--- a/Performance/Results.xlsx
+++ b/Performance/Results.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="1-16-2016" sheetId="1" r:id="rId1"/>
+    <sheet name="5-18-2016" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
   <si>
     <t>ReadTest1</t>
   </si>
@@ -49,14 +50,34 @@
   </si>
   <si>
     <t>Improvement</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Range (seconds)</t>
+  </si>
+  <si>
+    <t>WriteTest5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0%"/>
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -91,21 +112,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -198,6 +223,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -233,6 +275,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -387,7 +446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -643,4 +702,590 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B2" s="1">
+        <v>5005127507</v>
+      </c>
+      <c r="C2" s="1">
+        <v>737870677</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5038275699</v>
+      </c>
+      <c r="G2" s="1">
+        <v>239569427771</v>
+      </c>
+      <c r="H2" s="1">
+        <v>4502678826</v>
+      </c>
+      <c r="J2" s="1">
+        <v>2576434154</v>
+      </c>
+      <c r="L2">
+        <v>2579008764</v>
+      </c>
+      <c r="N2">
+        <v>2432804358</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>5041721143</v>
+      </c>
+      <c r="C3" s="1">
+        <v>738708353</v>
+      </c>
+      <c r="E3" s="1">
+        <v>5058628217</v>
+      </c>
+      <c r="H3" s="1">
+        <v>4513177010</v>
+      </c>
+      <c r="J3" s="1">
+        <v>2600901232</v>
+      </c>
+      <c r="L3">
+        <v>2581369020</v>
+      </c>
+      <c r="N3">
+        <v>2434521948</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>5049141007</v>
+      </c>
+      <c r="C4" s="1">
+        <v>741117953</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5074214827</v>
+      </c>
+      <c r="H4" s="1">
+        <v>4533586768</v>
+      </c>
+      <c r="J4" s="1">
+        <v>2603652297</v>
+      </c>
+      <c r="L4">
+        <v>2608444260</v>
+      </c>
+      <c r="N4">
+        <v>2436546660</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>5071920891</v>
+      </c>
+      <c r="C5" s="1">
+        <v>743811780</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5097346834</v>
+      </c>
+      <c r="H5" s="1">
+        <v>4551486658</v>
+      </c>
+      <c r="J5" s="1">
+        <v>2607466051</v>
+      </c>
+      <c r="L5">
+        <v>2608627428</v>
+      </c>
+      <c r="N5">
+        <v>2450578320</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>5116253750</v>
+      </c>
+      <c r="C6" s="1">
+        <v>745324886</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5135194615</v>
+      </c>
+      <c r="H6" s="1">
+        <v>4553663351</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2608073188</v>
+      </c>
+      <c r="L6">
+        <v>2608932180</v>
+      </c>
+      <c r="N6">
+        <v>2456242303</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>5158350307</v>
+      </c>
+      <c r="C7" s="1">
+        <v>745747671</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5145511605</v>
+      </c>
+      <c r="H7" s="1">
+        <v>4554869730</v>
+      </c>
+      <c r="J7" s="1">
+        <v>2612321965</v>
+      </c>
+      <c r="L7">
+        <v>2632283279</v>
+      </c>
+      <c r="N7">
+        <v>2459762750</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>5184841702</v>
+      </c>
+      <c r="C8" s="1">
+        <v>748467551</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5154588268</v>
+      </c>
+      <c r="H8" s="1">
+        <v>4574208511</v>
+      </c>
+      <c r="J8" s="1">
+        <v>2617320780</v>
+      </c>
+      <c r="L8">
+        <v>2641508369</v>
+      </c>
+      <c r="N8">
+        <v>2482953972</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>5203217275</v>
+      </c>
+      <c r="C9" s="1">
+        <v>775616612</v>
+      </c>
+      <c r="E9" s="1">
+        <v>5180162245</v>
+      </c>
+      <c r="H9" s="1">
+        <v>4584294569</v>
+      </c>
+      <c r="J9" s="1">
+        <v>2617466445</v>
+      </c>
+      <c r="L9">
+        <v>2642327886</v>
+      </c>
+      <c r="N9">
+        <v>2484008369</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>5266854966</v>
+      </c>
+      <c r="C10" s="1">
+        <v>792681588</v>
+      </c>
+      <c r="E10" s="1">
+        <v>5211061503</v>
+      </c>
+      <c r="H10" s="1">
+        <v>4619405495</v>
+      </c>
+      <c r="J10" s="1">
+        <v>2635412127</v>
+      </c>
+      <c r="L10">
+        <v>2665834123</v>
+      </c>
+      <c r="N10">
+        <v>2560211985</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>5285817149</v>
+      </c>
+      <c r="C11" s="1">
+        <v>806881415</v>
+      </c>
+      <c r="E11" s="1">
+        <v>5356003080</v>
+      </c>
+      <c r="H11" s="1">
+        <v>4770365151</v>
+      </c>
+      <c r="J11" s="1">
+        <v>2637111954</v>
+      </c>
+      <c r="L11">
+        <v>2730924523</v>
+      </c>
+      <c r="N11">
+        <v>2621384415</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1">
+        <f>MEDIAN(B2:B11)</f>
+        <v>5137302028.5</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" ref="C13:J13" si="0">MEDIAN(C2:C11)</f>
+        <v>745536278.5</v>
+      </c>
+      <c r="D13" s="4">
+        <f>($B13-C13)/$B13</f>
+        <v>0.85487785721687781</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" ref="E13" si="1">MEDIAN(E2:E11)</f>
+        <v>5140353110</v>
+      </c>
+      <c r="F13" s="5">
+        <f>($B13-E13)/$B13</f>
+        <v>-5.9390736286744287E-4</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="0"/>
+        <v>239569427771</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="0"/>
+        <v>4554266540.5</v>
+      </c>
+      <c r="I13" s="4">
+        <f>($G13-H13)/$G13</f>
+        <v>0.98098978411864246</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="0"/>
+        <v>2610197576.5</v>
+      </c>
+      <c r="K13" s="4">
+        <f>($G13-J13)/$G13</f>
+        <v>0.9891046299154872</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" ref="L13:N13" si="2">MEDIAN(L2:L11)</f>
+        <v>2620607729.5</v>
+      </c>
+      <c r="M13" s="4">
+        <f>($G13-L13)/$G13</f>
+        <v>0.98906117632002277</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="2"/>
+        <v>2458002526.5</v>
+      </c>
+      <c r="O13" s="4">
+        <f>($G13-N13)/$G13</f>
+        <v>0.98973991569220776</v>
+      </c>
+      <c r="P13" s="4">
+        <f>($J13-N13)/$J13</f>
+        <v>5.830786579921568E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3">
+        <f>B13/1000000000</f>
+        <v>5.1373020284999997</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" ref="C14:L14" si="3">C13/1000000000</f>
+        <v>0.74553627850000004</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3">
+        <f t="shared" si="3"/>
+        <v>5.1403531100000004</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3">
+        <f t="shared" si="3"/>
+        <v>239.56942777099999</v>
+      </c>
+      <c r="H14" s="3">
+        <f t="shared" si="3"/>
+        <v>4.5542665404999996</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3">
+        <f t="shared" si="3"/>
+        <v>2.6101975765000001</v>
+      </c>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3">
+        <f t="shared" si="3"/>
+        <v>2.6206077295000001</v>
+      </c>
+      <c r="N14" s="3">
+        <f t="shared" ref="N14:O14" si="4">N13/1000000000</f>
+        <v>2.4580025265000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="6">
+        <f>MIN(B2:B11)</f>
+        <v>5005127507</v>
+      </c>
+      <c r="C16" s="6">
+        <f>MIN(C2:C11)</f>
+        <v>737870677</v>
+      </c>
+      <c r="E16" s="6">
+        <f>MIN(E2:E11)</f>
+        <v>5038275699</v>
+      </c>
+      <c r="H16" s="6">
+        <f>MIN(H2:H11)</f>
+        <v>4502678826</v>
+      </c>
+      <c r="J16" s="6">
+        <f>MIN(J2:J11)</f>
+        <v>2576434154</v>
+      </c>
+      <c r="L16" s="6">
+        <f>MIN(L2:L11)</f>
+        <v>2579008764</v>
+      </c>
+      <c r="N16" s="6">
+        <f>MIN(N2:N11)</f>
+        <v>2432804358</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="6">
+        <f>MAX(B2:B11)</f>
+        <v>5285817149</v>
+      </c>
+      <c r="C17" s="6">
+        <f>MAX(C2:C11)</f>
+        <v>806881415</v>
+      </c>
+      <c r="E17" s="6">
+        <f>MAX(E2:E11)</f>
+        <v>5356003080</v>
+      </c>
+      <c r="H17" s="6">
+        <f>MAX(H2:H11)</f>
+        <v>4770365151</v>
+      </c>
+      <c r="J17" s="6">
+        <f>MAX(J2:J11)</f>
+        <v>2637111954</v>
+      </c>
+      <c r="L17" s="6">
+        <f>MAX(L2:L11)</f>
+        <v>2730924523</v>
+      </c>
+      <c r="N17" s="6">
+        <f>MAX(N2:N11)</f>
+        <v>2621384415</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="6">
+        <f>B17-B16</f>
+        <v>280689642</v>
+      </c>
+      <c r="C18" s="6">
+        <f>C17-C16</f>
+        <v>69010738</v>
+      </c>
+      <c r="E18" s="6">
+        <f>E17-E16</f>
+        <v>317727381</v>
+      </c>
+      <c r="H18" s="6">
+        <f>H17-H16</f>
+        <v>267686325</v>
+      </c>
+      <c r="J18" s="6">
+        <f>J17-J16</f>
+        <v>60677800</v>
+      </c>
+      <c r="L18" s="6">
+        <f>L17-L16</f>
+        <v>151915759</v>
+      </c>
+      <c r="N18" s="6">
+        <f>N17-N16</f>
+        <v>188580057</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="3">
+        <f>B18/1000000000</f>
+        <v>0.28068964200000002</v>
+      </c>
+      <c r="C19" s="3">
+        <f>C18/1000000000</f>
+        <v>6.9010738000000002E-2</v>
+      </c>
+      <c r="E19" s="3">
+        <f>E18/1000000000</f>
+        <v>0.31772738099999998</v>
+      </c>
+      <c r="H19" s="3">
+        <f>H18/1000000000</f>
+        <v>0.267686325</v>
+      </c>
+      <c r="J19" s="3">
+        <f>J18/1000000000</f>
+        <v>6.0677799999999997E-2</v>
+      </c>
+      <c r="L19" s="3">
+        <f>L18/1000000000</f>
+        <v>0.15191575900000001</v>
+      </c>
+      <c r="N19" s="3">
+        <f>N18/1000000000</f>
+        <v>0.188580057</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="7">
+        <f>B18/B13</f>
+        <v>5.4637558867053092E-2</v>
+      </c>
+      <c r="C20" s="7">
+        <f>C18/C13</f>
+        <v>9.2565231216980945E-2</v>
+      </c>
+      <c r="E20" s="7">
+        <f>E18/E13</f>
+        <v>6.1810419284600467E-2</v>
+      </c>
+      <c r="H20" s="7">
+        <f>H18/H13</f>
+        <v>5.8777044035418155E-2</v>
+      </c>
+      <c r="J20" s="7">
+        <f>J18/J13</f>
+        <v>2.3246439482700977E-2</v>
+      </c>
+      <c r="L20" s="7">
+        <f>L18/L13</f>
+        <v>5.7969667604157157E-2</v>
+      </c>
+      <c r="N20" s="7">
+        <f>N18/N13</f>
+        <v>7.6720855640666483E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="D13:M14 N13" formula="1"/>
+    <ignoredError sqref="D17 D16" formulaRange="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>